<commit_message>
update raw data on arm-init mg
</commit_message>
<xml_diff>
--- a/npb/data/asplos2023/asplos-unicifo.xlsx
+++ b/npb/data/asplos2023/asplos-unicifo.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26405"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{03F0B80D-4DED-4F40-9CCE-238B6794948B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{13B77D06-0E07-4766-82C5-8B9A0BFBDE7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -830,7 +830,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D11"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -961,9 +961,6 @@
       <c r="I4">
         <v>36.775999999999897</v>
       </c>
-      <c r="J4">
-        <v>296.02999999999997</v>
-      </c>
     </row>
     <row r="5" spans="1:11">
       <c r="A5" t="s">
@@ -1179,7 +1176,7 @@
       </c>
       <c r="D11">
         <f>J11/K11</f>
-        <v>0.83884178253288399</v>
+        <v>1.0101248887357901</v>
       </c>
       <c r="F11">
         <f>GEOMEAN(F1:F10)</f>
@@ -1199,7 +1196,7 @@
       </c>
       <c r="J11">
         <f>GEOMEAN(J1:J10)</f>
-        <v>1086.9281775914478</v>
+        <v>1308.8680455784468</v>
       </c>
       <c r="K11">
         <f>GEOMEAN(K1:K10)</f>

</xml_diff>